<commit_message>
moving files and model with nan substitution
</commit_message>
<xml_diff>
--- a/models/results_internal_external.xlsx
+++ b/models/results_internal_external.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">RF, null=-1, no class balancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF, null=median, no class balancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF, null=mean, no class balancing</t>
   </si>
   <si>
     <t xml:space="preserve">RF, null managed with RF, no class balancing</t>
@@ -47,10 +53,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -77,21 +84,14 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -138,7 +138,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -147,16 +147,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -176,22 +184,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -208,36 +217,69 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>0.8402</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>0.00389</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="4" t="n">
         <v>0.843202</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="5" t="n">
+        <v>0.838847926</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.00432671898687496</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.840236824150493</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.00455476898471562</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0.841631</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="n">
         <v>0.8394</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D5" s="4" t="n">
         <v>0.00277</v>
       </c>
+      <c r="E5" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
model with class balancing added
</commit_message>
<xml_diff>
--- a/models/results_internal_external.xlsx
+++ b/models/results_internal_external.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -37,16 +37,28 @@
     <t xml:space="preserve">external AUC</t>
   </si>
   <si>
-    <t xml:space="preserve">RF, null=-1, no class balancing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF, null=median, no class balancing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF, null=mean, no class balancing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF, null managed with RF, no class balancing</t>
+    <t xml:space="preserve">RF 100, null=-1, no class balancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF 100, null=median, no class balancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF 100, null=mean, no class balancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF 100, null managed with RF, no class balancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF 100, null=-1, balancing = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF 100, null=-1, balancing = 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF 100, null=-1, balancing = 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF 100, null=-1, balancing = 10</t>
   </si>
 </sst>
 </file>
@@ -138,7 +150,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -165,6 +177,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -184,10 +204,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -281,6 +301,66 @@
       </c>
       <c r="E5" s="4"/>
     </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.851611969901</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0.00372126517529</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0.863359</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.851354124315</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>0.00380425264735</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0.849760872926</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0.00438273660367</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.843638300354</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>0.00264344442622</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>